<commit_message>
Início da revisão do product backlog.
</commit_message>
<xml_diff>
--- a/Doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
+++ b/Doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Product-Backlog" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product-Backlog'!$A$1:$I$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product-Backlog'!$A$1:$I$94</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>Story Point</t>
   </si>
@@ -77,12 +77,6 @@
     <t>mobile/Web</t>
   </si>
   <si>
-    <t>Como Usuário, gostaria de Manter comodo</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de consultar os Relatórios de tempo de atividade do dispositivo</t>
-  </si>
-  <si>
     <t>Como Usuário, gostaria de consultar os Relatório de log de atividades</t>
   </si>
   <si>
@@ -107,18 +101,6 @@
     <t>Como Usuário, gostaria de logar</t>
   </si>
   <si>
-    <t>Como Usuário, gostaria de incluir residência.</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de excluir residência.</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de editar residência.</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de consultar residência.</t>
-  </si>
-  <si>
     <t>Como Usuário, gostaria de incluir cenario</t>
   </si>
   <si>
@@ -131,15 +113,6 @@
     <t>Como Usuário, gostaria de consultar cenario.</t>
   </si>
   <si>
-    <t>Como Usuário, gostaria de excluir dispositivos.</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de editar dispositivos.</t>
-  </si>
-  <si>
-    <t>Como Usuário, gostaria de consultar dispositivos.</t>
-  </si>
-  <si>
     <t>Como Usuário, gostaria de incluir usuário</t>
   </si>
   <si>
@@ -176,17 +149,53 @@
     <t>Como Usuário, gostaria de gerenciar dispositivos favoritos</t>
   </si>
   <si>
-    <t>Como usuário, gostaria de incluir dispositivos.</t>
-  </si>
-  <si>
     <t>Como Usuário, gostaria de gerenciar níveis de acesso ao dispositivo</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de incluir residência.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de excluir residência.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de editar residência.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de consultar residência.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de incluir Ambiente</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de editar Ambiente</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de excluir Ambiente</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de consultar Ambiente</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de incluir dispositivos.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de excluir dispositivos.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de editar dispositivos.</t>
+  </si>
+  <si>
+    <t>Como Administrador, gostaria de consultar dispositivos.</t>
+  </si>
+  <si>
+    <t>Como Usuário, gostaria de consultar os relatórios de tempo de atividade do dispositivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +228,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -339,6 +355,12 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,11 +935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1020,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1009,13 +1031,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1026,13 +1048,13 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1043,13 +1065,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1060,13 +1082,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1077,13 +1099,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1097,13 +1119,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1115,13 +1137,13 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1133,13 +1155,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1151,13 +1173,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1169,13 +1191,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1187,13 +1209,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1205,13 +1227,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1223,13 +1245,13 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1241,13 +1263,13 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>40</v>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1255,19 +1277,17 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="15"/>
-      <c r="R16" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>41</v>
+      <c r="C17" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1279,13 +1299,13 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>42</v>
+      <c r="C18" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1297,13 +1317,13 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1311,17 +1331,19 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="15"/>
-      <c r="R19" s="12"/>
+      <c r="R19" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1329,19 +1351,17 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="15"/>
-      <c r="R20" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="R20" s="12"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1353,71 +1373,69 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>25</v>
-      </c>
-      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="14"/>
-      <c r="R22" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="C22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="15"/>
+      <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>26</v>
-      </c>
-      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="14"/>
+      <c r="C23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="15"/>
       <c r="R23" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>27</v>
-      </c>
-      <c r="B24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="14"/>
+      <c r="C24" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="15"/>
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>49</v>
+      <c r="C25" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1425,17 +1443,19 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="14"/>
-      <c r="R25" s="12"/>
+      <c r="R25" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1443,132 +1463,131 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="14"/>
-      <c r="R26" s="12"/>
-    </row>
-    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="R26" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="15"/>
+      <c r="C27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="14"/>
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="15"/>
-      <c r="R28" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="C28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="14"/>
+      <c r="R28" s="12"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="15"/>
-      <c r="R29" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="C29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="14"/>
+      <c r="R29" s="12"/>
     </row>
     <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>31</v>
-      </c>
-      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="14"/>
-      <c r="R30" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="15"/>
+      <c r="R30" s="12"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="15"/>
       <c r="R31" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>33</v>
-      </c>
-      <c r="B32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="15"/>
+      <c r="R32" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1576,16 +1595,19 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="14"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R33" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1593,16 +1615,19 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="14"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R34" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1611,15 +1636,15 @@
       <c r="H35" s="2"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1628,64 +1653,75 @@
       <c r="H36" s="2"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>38</v>
-      </c>
-      <c r="B37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="15"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>39</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>40</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="14"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>41</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C40" s="8"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="15"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <f t="shared" ref="A41:A84" si="1">A40+1</f>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="8"/>
@@ -1696,10 +1732,9 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <f t="shared" si="1"/>
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="8"/>
@@ -1710,10 +1745,9 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="8"/>
@@ -1724,10 +1758,9 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="8"/>
@@ -1738,10 +1771,9 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="8"/>
@@ -1752,10 +1784,9 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="8"/>
@@ -1766,24 +1797,22 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="8"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="3"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <f t="shared" si="1"/>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="8"/>
@@ -1796,92 +1825,85 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="B49" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="B49" s="2"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B50" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="B50" s="2"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="B51" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B51" s="2"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="B52" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="B52" s="5"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="B53" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="B53" s="5"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="B54" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="B54" s="5"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <f t="shared" si="1"/>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="8"/>
@@ -1894,8 +1916,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <f t="shared" si="1"/>
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="8"/>
@@ -1908,8 +1929,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <f t="shared" si="1"/>
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="8"/>
@@ -1922,50 +1942,46 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="B58" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B58" s="2"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="B59" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="2"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="B60" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="B60" s="2"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <f t="shared" si="1"/>
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="8"/>
@@ -1978,8 +1994,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <f t="shared" si="1"/>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="8"/>
@@ -1992,8 +2007,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <f t="shared" si="1"/>
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="8"/>
@@ -2006,22 +2020,20 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="B64" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="B64" s="5"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <f t="shared" si="1"/>
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="8"/>
@@ -2034,8 +2046,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <f t="shared" si="1"/>
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="8"/>
@@ -2048,8 +2059,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <f t="shared" si="1"/>
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="8"/>
@@ -2062,36 +2072,33 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B68" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B68" s="5"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B69" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B69" s="5"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="8"/>
@@ -2104,22 +2111,20 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B71" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="B71" s="2"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <f t="shared" si="1"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="8"/>
@@ -2132,8 +2137,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <f t="shared" si="1"/>
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="8"/>
@@ -2146,8 +2150,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <f t="shared" si="1"/>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="8"/>
@@ -2160,8 +2163,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <f t="shared" si="1"/>
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="8"/>
@@ -2174,8 +2176,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <f t="shared" si="1"/>
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="8"/>
@@ -2188,8 +2189,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <f t="shared" si="1"/>
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="8"/>
@@ -2202,50 +2202,46 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B78" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="B78" s="2"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B79" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B79" s="2"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B80" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B80" s="5"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <f t="shared" si="1"/>
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="8"/>
@@ -2258,8 +2254,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <f t="shared" si="1"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="8"/>
@@ -2272,22 +2267,20 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B83" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="B83" s="2"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <f t="shared" si="1"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="8"/>
@@ -2297,12 +2290,10 @@
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
-      <c r="N84" s="4"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <f t="shared" ref="A85:A89" si="2">A84+1</f>
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="8"/>
@@ -2315,8 +2306,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <f t="shared" si="2"/>
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="8"/>
@@ -2329,8 +2319,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <f t="shared" si="2"/>
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="8"/>
@@ -2340,50 +2329,88 @@
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
+      <c r="N87" s="4"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <f t="shared" si="2"/>
-        <v>89</v>
-      </c>
-      <c r="B88" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="B88" s="5"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="B89" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B89" s="5"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="6">
-        <v>76</v>
-      </c>
-      <c r="B90" s="6"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="6"/>
-      <c r="I90" s="6"/>
+      <c r="A90" s="2">
+        <v>86</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>87</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>88</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>89</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E49:E51">
+  <conditionalFormatting sqref="E52:E54">
     <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>$P$1</formula>
     </cfRule>
@@ -2403,7 +2430,7 @@
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E76">
+  <conditionalFormatting sqref="E61:E79">
     <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
       <formula>$P$1</formula>
     </cfRule>
@@ -2423,7 +2450,7 @@
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:E79">
+  <conditionalFormatting sqref="E80:E82">
     <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>$P$1</formula>
     </cfRule>
@@ -2443,7 +2470,7 @@
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E87">
+  <conditionalFormatting sqref="E88:E90">
     <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>$P$1</formula>
     </cfRule>
@@ -2463,7 +2490,7 @@
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88:E90">
+  <conditionalFormatting sqref="E91:E93">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$P$1</formula>
     </cfRule>
@@ -2483,7 +2510,7 @@
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E90">
+  <conditionalFormatting sqref="E2:E93">
     <cfRule type="cellIs" dxfId="5" priority="61" operator="equal">
       <formula>$K$1</formula>
     </cfRule>
@@ -2504,17 +2531,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E85:E90 E2:E82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E88:E93 E2:E85">
       <formula1>$K$1:$P$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G93">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I90">
-      <formula1>$R$7:$R$23</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I93">
+      <formula1>$R$7:$R$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B90">
-      <formula1>$R$28:$R$31</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B93">
+      <formula1>$R$31:$R$34</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionando o backlog alterado em sala
</commit_message>
<xml_diff>
--- a/Doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
+++ b/Doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
@@ -95,9 +95,6 @@
     <t>Como Usuário, gostaria de incluir usuário</t>
   </si>
   <si>
-    <t>Como Usuário, gostaria de excluir usuario.</t>
-  </si>
-  <si>
     <t>Como Usuário, gostaria de editar usuário.</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Como Usuário, gostaria de receber push notification quando o dipositivo ultrapassar um tempo determinado de uso</t>
+  </si>
+  <si>
+    <t>Como Usuário(ADM Todos os perfis), gostaria de excluir usuario.</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -399,6 +399,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -977,8 +980,8 @@
   <dimension ref="A1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1081,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
@@ -1097,7 +1100,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -1116,7 +1119,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
@@ -1135,7 +1138,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
@@ -1154,7 +1157,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5">
@@ -1176,7 +1179,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5">
@@ -1196,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5">
@@ -1216,7 +1219,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5">
@@ -1236,7 +1239,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5">
@@ -1256,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5">
@@ -1276,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5">
@@ -1296,7 +1299,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5">
@@ -1316,7 +1319,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5">
@@ -1336,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5">
@@ -1356,7 +1359,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5">
@@ -1376,7 +1379,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5">
@@ -1396,7 +1399,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5">
@@ -1416,7 +1419,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5">
@@ -1436,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5">
@@ -1456,7 +1459,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5">
@@ -1476,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5">
@@ -1496,7 +1499,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5">
@@ -1516,7 +1519,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5">
@@ -1536,7 +1539,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5">
@@ -1556,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5">
@@ -1576,7 +1579,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5">
@@ -1596,7 +1599,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5">
@@ -1616,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5">
@@ -1636,7 +1639,7 @@
         <v>14</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5">
@@ -1677,8 +1680,8 @@
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>25</v>
+      <c r="C33" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5">
@@ -1697,8 +1700,8 @@
       <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>26</v>
+      <c r="C34" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5">
@@ -1717,8 +1720,8 @@
       <c r="B35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>27</v>
+      <c r="C35" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5">
@@ -1737,7 +1740,7 @@
       <c r="B36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="5"/>
@@ -1757,7 +1760,7 @@
       <c r="B37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D37" s="5"/>
@@ -1777,7 +1780,7 @@
       <c r="B38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="5"/>
@@ -1797,7 +1800,7 @@
       <c r="B39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="5"/>
@@ -1818,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5">
@@ -1840,7 +1843,7 @@
         <v>18</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5">
@@ -1860,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2">
@@ -1882,7 +1885,7 @@
         <v>18</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2">
@@ -1904,7 +1907,7 @@
         <v>18</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2">
@@ -1924,7 +1927,7 @@
         <v>18</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2">
@@ -1944,7 +1947,7 @@
         <v>18</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2">
@@ -1964,7 +1967,7 @@
         <v>18</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5">
@@ -1984,7 +1987,7 @@
         <v>18</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5">
@@ -2006,7 +2009,7 @@
         <v>18</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5">
@@ -2028,7 +2031,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2">
@@ -2050,7 +2053,7 @@
         <v>18</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2">
@@ -2072,7 +2075,7 @@
         <v>18</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2">
@@ -2091,7 +2094,7 @@
         <v>15</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2">

</xml_diff>